<commit_message>
Updated model selection results for RMR and SMR
</commit_message>
<xml_diff>
--- a/results/RMR results/gamm_RMR_model_selection.xlsx
+++ b/results/RMR results/gamm_RMR_model_selection.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">model</t>
   </si>
@@ -104,6 +104,12 @@
     <t xml:space="preserve">m1</t>
   </si>
   <si>
+    <t xml:space="preserve">mean_rmr ~ s(doy_id, bs = "cc", k = 20) + ti(doy_id, fish_basin, bs = c("cc", "fs"), k = c(20, 3))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m12</t>
+  </si>
+  <si>
     <t xml:space="preserve">mean_rmr ~ s(doy_id, by = fish_basin, bs = "cc", k = 20) + ti(doy_id, fish_basin, bs = c("cc", "fs"), k = c(20, 3))</t>
   </si>
   <si>
@@ -120,6 +126,9 @@
   </si>
   <si>
     <t xml:space="preserve">m6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m13</t>
   </si>
   <si>
     <t xml:space="preserve">mean_rmr ~ s(floy_tag, year, by = fish_basin, bs = c("re", "re"), k = c(20, 4))</t>
@@ -503,7 +512,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="n">
-        <v>64.9510094809457</v>
+        <v>64.9510094809466</v>
       </c>
       <c r="D2" t="n">
         <v>-12198.3745868277</v>
@@ -515,13 +524,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0.99714799578385</v>
+        <v>0.99714799578383</v>
       </c>
       <c r="H2" t="n">
         <v>24933.8230148604</v>
       </c>
       <c r="I2" t="n">
-        <v>64.2012336222773</v>
+        <v>64.2012336222772</v>
       </c>
       <c r="J2" t="n">
         <v>3106.04899051905</v>
@@ -535,7 +544,7 @@
         <v>13</v>
       </c>
       <c r="C3" t="n">
-        <v>59.6408853147914</v>
+        <v>59.6408853147918</v>
       </c>
       <c r="D3" t="n">
         <v>-12208.9561357818</v>
@@ -544,16 +553,16 @@
         <v>24542.8802636212</v>
       </c>
       <c r="F3" t="n">
-        <v>12.8919399804108</v>
+        <v>12.8919399803963</v>
       </c>
       <c r="G3" t="n">
-        <v>0.00158237868198908</v>
+        <v>0.00158237868200056</v>
       </c>
       <c r="H3" t="n">
         <v>24921.645892871</v>
       </c>
       <c r="I3" t="n">
-        <v>64.6512160563653</v>
+        <v>64.6512160563652</v>
       </c>
       <c r="J3" t="n">
         <v>3111.35911468521</v>
@@ -576,16 +585,16 @@
         <v>24543.3206780369</v>
       </c>
       <c r="F4" t="n">
-        <v>13.3323543961051</v>
+        <v>13.3323543960905</v>
       </c>
       <c r="G4" t="n">
-        <v>0.00126962553416011</v>
+        <v>0.00126962553416932</v>
       </c>
       <c r="H4" t="n">
         <v>24921.9695369114</v>
       </c>
       <c r="I4" t="n">
-        <v>64.6610879511879</v>
+        <v>64.6610879511878</v>
       </c>
       <c r="J4" t="n">
         <v>3111.39705357782</v>
@@ -599,7 +608,7 @@
         <v>17</v>
       </c>
       <c r="C5" t="n">
-        <v>65.6832608957113</v>
+        <v>65.6832608957114</v>
       </c>
       <c r="D5" t="n">
         <v>-12233.3669886678</v>
@@ -608,10 +617,10 @@
         <v>24600.8238656186</v>
       </c>
       <c r="F5" t="n">
-        <v>70.8355419777799</v>
+        <v>70.8355419777945</v>
       </c>
       <c r="G5" t="n">
-        <v>0.000000000000000414015994059663</v>
+        <v>0.000000000000000414015994056642</v>
       </c>
       <c r="H5" t="n">
         <v>25007.2370605122</v>
@@ -631,7 +640,7 @@
         <v>19</v>
       </c>
       <c r="C6" t="n">
-        <v>60.8896591714629</v>
+        <v>60.8896591714626</v>
       </c>
       <c r="D6" t="n">
         <v>-12241.7476688094</v>
@@ -640,10 +649,10 @@
         <v>24610.8264681318</v>
       </c>
       <c r="F6" t="n">
-        <v>80.8381444910046</v>
+        <v>80.8381444910119</v>
       </c>
       <c r="G6" t="n">
-        <v>0.00000000000000000278599017686958</v>
+        <v>0.00000000000000000278599017685939</v>
       </c>
       <c r="H6" t="n">
         <v>24996.7545364133</v>
@@ -663,7 +672,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="n">
-        <v>60.9188421216228</v>
+        <v>60.9188421216227</v>
       </c>
       <c r="D7" t="n">
         <v>-12241.7590319836</v>
@@ -672,10 +681,10 @@
         <v>24610.876539338</v>
       </c>
       <c r="F7" t="n">
-        <v>80.8882156971631</v>
+        <v>80.8882156971558</v>
       </c>
       <c r="G7" t="n">
-        <v>0.00000000000000000271710709521319</v>
+        <v>0.00000000000000000271710709522302</v>
       </c>
       <c r="H7" t="n">
         <v>24996.8874871802</v>
@@ -695,7 +704,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="n">
-        <v>32.770751056021</v>
+        <v>32.7707510560212</v>
       </c>
       <c r="D8" t="n">
         <v>-12440.5084103638</v>
@@ -707,7 +716,7 @@
         <v>419.151328637487</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000957646147399912</v>
+        <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000957646147399892</v>
       </c>
       <c r="H8" t="n">
         <v>25155.6132198997</v>
@@ -727,7 +736,7 @@
         <v>25</v>
       </c>
       <c r="C9" t="n">
-        <v>52.3901574368339</v>
+        <v>52.3901574368335</v>
       </c>
       <c r="D9" t="n">
         <v>-12755.1812568349</v>
@@ -736,10 +745,10 @@
         <v>25617.9493651229</v>
       </c>
       <c r="F9" t="n">
-        <v>1087.96104148204</v>
+        <v>1087.96104148203</v>
       </c>
       <c r="G9" t="n">
-        <v>5.63665170356948e-237</v>
+        <v>5.63665170361038e-237</v>
       </c>
       <c r="H9" t="n">
         <v>25944.0344755474</v>
@@ -759,7 +768,7 @@
         <v>27</v>
       </c>
       <c r="C10" t="n">
-        <v>52.048928187642</v>
+        <v>52.0489281876422</v>
       </c>
       <c r="D10" t="n">
         <v>-12756.3302759389</v>
@@ -768,10 +777,10 @@
         <v>25619.5493696745</v>
       </c>
       <c r="F10" t="n">
-        <v>1089.56104603367</v>
+        <v>1089.56104603368</v>
       </c>
       <c r="G10" t="n">
-        <v>2.53270510708389e-237</v>
+        <v>2.53270510707462e-237</v>
       </c>
       <c r="H10" t="n">
         <v>25943.5188090962</v>
@@ -791,25 +800,25 @@
         <v>29</v>
       </c>
       <c r="C11" t="n">
-        <v>46.4354984461214</v>
+        <v>46.4354984461203</v>
       </c>
       <c r="D11" t="n">
-        <v>-12764.4243811726</v>
+        <v>-12764.4243811727</v>
       </c>
       <c r="E11" t="n">
-        <v>25626.5628256412</v>
+        <v>25626.5628256413</v>
       </c>
       <c r="F11" t="n">
-        <v>1096.57450200041</v>
+        <v>1096.57450200044</v>
       </c>
       <c r="G11" t="n">
-        <v>7.59682309770468e-239</v>
+        <v>7.5968230976078e-239</v>
       </c>
       <c r="H11" t="n">
-        <v>25922.7244912121</v>
+        <v>25922.7244912122</v>
       </c>
       <c r="I11" t="n">
-        <v>89.0046531657699</v>
+        <v>89.0046531657701</v>
       </c>
       <c r="J11" t="n">
         <v>3124.56450155388</v>
@@ -823,28 +832,28 @@
         <v>31</v>
       </c>
       <c r="C12" t="n">
-        <v>50.2222353527672</v>
+        <v>46.0793257968961</v>
       </c>
       <c r="D12" t="n">
-        <v>-12781.3669418282</v>
+        <v>-12783.764126557</v>
       </c>
       <c r="E12" t="n">
-        <v>25666.0173089854</v>
+        <v>25663.6677836898</v>
       </c>
       <c r="F12" t="n">
-        <v>1136.02898534461</v>
+        <v>1133.67946004902</v>
       </c>
       <c r="G12" t="n">
-        <v>2.05683669636695e-247</v>
+        <v>6.65875057825933e-247</v>
       </c>
       <c r="H12" t="n">
-        <v>25979.0591602763</v>
+        <v>25955.0571962489</v>
       </c>
       <c r="I12" t="n">
-        <v>89.9453597069725</v>
+        <v>90.0850890575436</v>
       </c>
       <c r="J12" t="n">
-        <v>3120.77776464723</v>
+        <v>3124.9206742031</v>
       </c>
     </row>
     <row r="13">
@@ -855,28 +864,28 @@
         <v>33</v>
       </c>
       <c r="C13" t="n">
-        <v>44.3735763128742</v>
+        <v>50.2222353527666</v>
       </c>
       <c r="D13" t="n">
-        <v>-12790.9423644334</v>
+        <v>-12781.3669418282</v>
       </c>
       <c r="E13" t="n">
-        <v>25675.4615084122</v>
+        <v>25666.0173089854</v>
       </c>
       <c r="F13" t="n">
-        <v>1145.47318477132</v>
+        <v>1136.02898534459</v>
       </c>
       <c r="G13" t="n">
-        <v>1.82986042037731e-249</v>
+        <v>2.05683669638188e-247</v>
       </c>
       <c r="H13" t="n">
-        <v>25959.083475958</v>
+        <v>25979.0591602762</v>
       </c>
       <c r="I13" t="n">
-        <v>90.4979694636369</v>
+        <v>89.9453597069725</v>
       </c>
       <c r="J13" t="n">
-        <v>3126.62642368713</v>
+        <v>3120.77776464723</v>
       </c>
     </row>
     <row r="14">
@@ -887,28 +896,28 @@
         <v>35</v>
       </c>
       <c r="C14" t="n">
-        <v>17.8541139722697</v>
+        <v>44.3735763128743</v>
       </c>
       <c r="D14" t="n">
-        <v>-13011.7192333895</v>
+        <v>-12790.9423644334</v>
       </c>
       <c r="E14" t="n">
-        <v>26061.6464039788</v>
+        <v>25675.4615084122</v>
       </c>
       <c r="F14" t="n">
-        <v>1531.65808033794</v>
+        <v>1145.47318477132</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1.82986042037727e-249</v>
       </c>
       <c r="H14" t="n">
-        <v>26177.4508842902</v>
+        <v>25959.083475958</v>
       </c>
       <c r="I14" t="n">
-        <v>103.963639832768</v>
+        <v>90.4979694636369</v>
       </c>
       <c r="J14" t="n">
-        <v>3153.14588602773</v>
+        <v>3126.62642368713</v>
       </c>
     </row>
     <row r="15">
@@ -919,59 +928,123 @@
         <v>37</v>
       </c>
       <c r="C15" t="n">
-        <v>15.7334421526263</v>
+        <v>17.8541139722698</v>
       </c>
       <c r="D15" t="n">
-        <v>-13255.5300900255</v>
+        <v>-13011.7192333895</v>
       </c>
       <c r="E15" t="n">
-        <v>26544.7858060008</v>
+        <v>26061.6464039788</v>
       </c>
       <c r="F15" t="n">
-        <v>2014.79748235998</v>
+        <v>1531.65808033794</v>
       </c>
       <c r="G15" t="n">
         <v>0</v>
       </c>
       <c r="H15" t="n">
-        <v>26647.004844047</v>
+        <v>26177.4508842902</v>
       </c>
       <c r="I15" t="n">
-        <v>121.055090872987</v>
+        <v>103.963639832768</v>
       </c>
       <c r="J15" t="n">
-        <v>3155.26655784737</v>
+        <v>3153.14588602773</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
-        <v>39</v>
-      </c>
       <c r="C16" t="n">
-        <v>3</v>
+        <v>17.8541139722698</v>
       </c>
       <c r="D16" t="n">
-        <v>-13740.8325028266</v>
+        <v>-13011.7192333895</v>
       </c>
       <c r="E16" t="n">
-        <v>27489.6650056532</v>
+        <v>26061.6464039788</v>
       </c>
       <c r="F16" t="n">
-        <v>2959.67668201236</v>
+        <v>1531.65808033794</v>
       </c>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
+        <v>26177.4508842902</v>
+      </c>
+      <c r="I16" t="n">
+        <v>103.963639832768</v>
+      </c>
+      <c r="J16" t="n">
+        <v>3153.14588602773</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" t="n">
+        <v>15.7334421526262</v>
+      </c>
+      <c r="D17" t="n">
+        <v>-13255.5300900255</v>
+      </c>
+      <c r="E17" t="n">
+        <v>26544.7858060008</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2014.79748235998</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+      <c r="H17" t="n">
+        <v>26647.004844047</v>
+      </c>
+      <c r="I17" t="n">
+        <v>121.055090872987</v>
+      </c>
+      <c r="J17" t="n">
+        <v>3155.26655784737</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C18" t="n">
+        <v>3</v>
+      </c>
+      <c r="D18" t="n">
+        <v>-13740.8325028266</v>
+      </c>
+      <c r="E18" t="n">
+        <v>27489.6650056531</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2959.6766820123</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+      <c r="H18" t="n">
         <v>27513.9122147513</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I18" t="n">
         <v>164.152552938107</v>
       </c>
-      <c r="J16" t="n">
+      <c r="J18" t="n">
         <v>3168</v>
       </c>
     </row>

</xml_diff>